<commit_message>
Added tests for universal tabular form setting.
</commit_message>
<xml_diff>
--- a/EPPlusTest/Workbooks/PivotTables/PivotTableTabularSettingsEnabled.xlsx
+++ b/EPPlusTest/Workbooks/PivotTables/PivotTableTabularSettingsEnabled.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\source\EPPlus\EPPlusTest\Workbooks\PivotTables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{926A056E-A331-4F04-9BDD-D26BC29A80DB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA5503B2-58F6-4C1F-BE1C-722AF0678710}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20688" windowHeight="8880" activeTab="3" xr2:uid="{E88C8B23-488D-4841-895F-A0AE7CD751FD}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20688" windowHeight="8880" activeTab="4" xr2:uid="{E88C8B23-488D-4841-895F-A0AE7CD751FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="TwoTabularFields" sheetId="2" r:id="rId2"/>
     <sheet name="ThreeTabularFields" sheetId="3" r:id="rId3"/>
     <sheet name="FourTabularFields" sheetId="4" r:id="rId4"/>
+    <sheet name="PivotTables" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="76" r:id="rId5"/>
+    <pivotCache cacheId="14" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="53">
   <si>
     <t>Transaction</t>
   </si>
@@ -183,6 +184,18 @@
   </si>
   <si>
     <t>Tabular Second And Third Fields</t>
+  </si>
+  <si>
+    <t>Sum of Units Sold</t>
+  </si>
+  <si>
+    <t>Total Sum of Units Sold</t>
+  </si>
+  <si>
+    <t>Total Sum of Total</t>
+  </si>
+  <si>
+    <t>Values</t>
   </si>
 </sst>
 </file>
@@ -426,21 +439,10 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9489D35E-5C73-42E5-85C8-4C22966D7885}" name="PivotTable3" cacheId="76" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A19:N32" firstHeaderRow="1" firstDataRow="3" firstDataCol="2"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C85503F4-685C-4E34-9D3D-85E927BBC202}" name="PivotTable2" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="F2:L14" firstHeaderRow="1" firstDataRow="2" firstDataCol="2"/>
   <pivotFields count="7">
-    <pivotField axis="axisCol" showAll="0">
-      <items count="8">
-        <item x="3"/>
-        <item x="5"/>
-        <item x="4"/>
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item x="6"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
+    <pivotField showAll="0"/>
     <pivotField axis="axisRow" outline="0" showAll="0">
       <items count="4">
         <item x="1"/>
@@ -512,46 +514,20 @@
       <x/>
     </i>
   </rowItems>
-  <colFields count="2">
+  <colFields count="1">
     <field x="3"/>
-    <field x="0"/>
   </colFields>
-  <colItems count="12">
-    <i>
-      <x/>
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="3"/>
-    </i>
-    <i r="1">
-      <x v="6"/>
-    </i>
-    <i t="default">
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-      <x v="4"/>
-    </i>
-    <i t="default">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-      <x v="5"/>
-    </i>
-    <i t="default">
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-      <x v="2"/>
-    </i>
-    <i t="default">
+  <colItems count="5">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
       <x v="3"/>
     </i>
     <i t="grand">
@@ -574,200 +550,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable10.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{86510E5D-205D-4903-98AE-6E2D516E3FAC}" name="PivotTable6" cacheId="76" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="G71:M101" firstHeaderRow="1" firstDataRow="2" firstDataCol="3"/>
-  <pivotFields count="7">
-    <pivotField axis="axisRow" showAll="0">
-      <items count="8">
-        <item x="3"/>
-        <item x="5"/>
-        <item x="4"/>
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item x="6"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" outline="0" showAll="0">
-      <items count="4">
-        <item x="1"/>
-        <item x="2"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" outline="0" showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="5">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField numFmtId="8" showAll="0"/>
-    <pivotField axis="axisCol" showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" numFmtId="8" showAll="0"/>
-  </pivotFields>
-  <rowFields count="4">
-    <field x="0"/>
-    <field x="1"/>
-    <field x="2"/>
-    <field x="3"/>
-  </rowFields>
-  <rowItems count="29">
-    <i>
-      <x/>
-    </i>
-    <i r="1">
-      <x/>
-      <x/>
-      <x/>
-    </i>
-    <i t="default" r="2">
-      <x/>
-    </i>
-    <i t="default" r="1">
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-      <x v="2"/>
-      <x/>
-    </i>
-    <i t="default" r="2">
-      <x v="2"/>
-    </i>
-    <i t="default" r="1">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-      <x v="1"/>
-      <x v="3"/>
-    </i>
-    <i t="default" r="2">
-      <x v="1"/>
-    </i>
-    <i t="default" r="1">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i r="1">
-      <x v="2"/>
-      <x/>
-      <x/>
-    </i>
-    <i t="default" r="2">
-      <x/>
-    </i>
-    <i t="default" r="1">
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i r="1">
-      <x/>
-      <x v="2"/>
-      <x v="1"/>
-    </i>
-    <i t="default" r="2">
-      <x v="2"/>
-    </i>
-    <i t="default" r="1">
-      <x/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i r="1">
-      <x v="2"/>
-      <x v="1"/>
-      <x v="2"/>
-    </i>
-    <i t="default" r="2">
-      <x v="1"/>
-    </i>
-    <i t="default" r="1">
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-      <x/>
-      <x/>
-    </i>
-    <i t="default" r="2">
-      <x/>
-    </i>
-    <i t="default" r="1">
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="5"/>
-  </colFields>
-  <colItems count="4">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable11.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A96AE210-2FEB-4A36-8C77-5733153C79A5}" name="PivotTable5" cacheId="76" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A96AE210-2FEB-4A36-8C77-5733153C79A5}" name="PivotTable5" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A71:D100" firstHeaderRow="1" firstDataRow="1" firstDataCol="3"/>
   <pivotFields count="7">
     <pivotField axis="axisRow" showAll="0">
@@ -938,8 +721,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable12.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F5D0F6D2-18CC-4201-8818-EC7141389A69}" name="PivotTable4" cacheId="76" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<file path=xl/pivotTables/pivotTable11.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F5D0F6D2-18CC-4201-8818-EC7141389A69}" name="PivotTable4" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="G37:M67" firstHeaderRow="1" firstDataRow="2" firstDataCol="3"/>
   <pivotFields count="7">
     <pivotField axis="axisRow" outline="0" showAll="0">
@@ -1131,8 +914,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable13.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{582D5AD1-5934-41D2-B10D-A3BDAE90505D}" name="PivotTable3" cacheId="76" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<file path=xl/pivotTables/pivotTable12.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{582D5AD1-5934-41D2-B10D-A3BDAE90505D}" name="PivotTable3" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A37:D66" firstHeaderRow="1" firstDataRow="1" firstDataCol="3"/>
   <pivotFields count="7">
     <pivotField axis="axisRow" outline="0" showAll="0">
@@ -1303,8 +1086,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable14.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{EEA2CD44-3B8C-4BDE-B0D3-42BDE6F05390}" name="PivotTable2" cacheId="76" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<file path=xl/pivotTables/pivotTable13.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{EEA2CD44-3B8C-4BDE-B0D3-42BDE6F05390}" name="PivotTable2" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="G2:N32" firstHeaderRow="1" firstDataRow="2" firstDataCol="3"/>
   <pivotFields count="7">
     <pivotField axis="axisRow" outline="0" showAll="0">
@@ -1500,8 +1283,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable15.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F398EFCB-3E9D-4598-985E-313DB1616872}" name="PivotTable1" cacheId="76" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<file path=xl/pivotTables/pivotTable14.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F398EFCB-3E9D-4598-985E-313DB1616872}" name="PivotTable1" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A2:D31" firstHeaderRow="1" firstDataRow="1" firstDataCol="3"/>
   <pivotFields count="7">
     <pivotField axis="axisRow" outline="0" showAll="0">
@@ -1672,11 +1455,914 @@
 </pivotTableDefinition>
 </file>
 
+<file path=xl/pivotTables/pivotTable15.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{86510E5D-205D-4903-98AE-6E2D516E3FAC}" name="PivotTable6" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="G71:M101" firstHeaderRow="1" firstDataRow="2" firstDataCol="3"/>
+  <pivotFields count="7">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="8">
+        <item x="3"/>
+        <item x="5"/>
+        <item x="4"/>
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="6"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" outline="0" showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" outline="0" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField numFmtId="8" showAll="0"/>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" numFmtId="8" showAll="0"/>
+  </pivotFields>
+  <rowFields count="4">
+    <field x="0"/>
+    <field x="1"/>
+    <field x="2"/>
+    <field x="3"/>
+  </rowFields>
+  <rowItems count="29">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x/>
+      <x/>
+      <x/>
+    </i>
+    <i t="default" r="2">
+      <x/>
+    </i>
+    <i t="default" r="1">
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+      <x v="2"/>
+      <x/>
+    </i>
+    <i t="default" r="2">
+      <x v="2"/>
+    </i>
+    <i t="default" r="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+      <x v="1"/>
+      <x v="3"/>
+    </i>
+    <i t="default" r="2">
+      <x v="1"/>
+    </i>
+    <i t="default" r="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+      <x/>
+      <x/>
+    </i>
+    <i t="default" r="2">
+      <x/>
+    </i>
+    <i t="default" r="1">
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x/>
+      <x v="2"/>
+      <x v="1"/>
+    </i>
+    <i t="default" r="2">
+      <x v="2"/>
+    </i>
+    <i t="default" r="1">
+      <x/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+      <x v="1"/>
+      <x v="2"/>
+    </i>
+    <i t="default" r="2">
+      <x v="1"/>
+    </i>
+    <i t="default" r="1">
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+      <x/>
+      <x/>
+    </i>
+    <i t="default" r="2">
+      <x/>
+    </i>
+    <i t="default" r="1">
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="5"/>
+  </colFields>
+  <colItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable16.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0A51E118-939E-4F24-95AC-05D251CE4ABC}" name="PivotTable5" cacheId="14" dataPosition="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+  <location ref="A50:P61" firstHeaderRow="1" firstDataRow="4" firstDataCol="2"/>
+  <pivotFields count="7">
+    <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <items count="7">
+        <item x="3"/>
+        <item x="5"/>
+        <item x="4"/>
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="6"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+      </items>
+    </pivotField>
+    <pivotField compact="0" numFmtId="8" outline="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dataField="1" compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dataField="1" compact="0" numFmtId="8" outline="0" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="0"/>
+    <field x="2"/>
+  </rowFields>
+  <rowItems count="8">
+    <i>
+      <x/>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="2"/>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="3"/>
+      <x/>
+    </i>
+    <i>
+      <x v="4"/>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="5"/>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="6"/>
+      <x/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="3">
+    <field x="-2"/>
+    <field x="1"/>
+    <field x="3"/>
+  </colFields>
+  <colItems count="14">
+    <i>
+      <x/>
+      <x/>
+      <x/>
+    </i>
+    <i r="2">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+      <x/>
+    </i>
+    <i r="2">
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+      <x/>
+    </i>
+    <i r="2">
+      <x v="2"/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+      <x/>
+      <x/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+      <x/>
+    </i>
+    <i r="2" i="1">
+      <x v="3"/>
+    </i>
+    <i r="1" i="1">
+      <x v="2"/>
+      <x/>
+    </i>
+    <i r="2" i="1">
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+    <i t="grand" i="1">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Units Sold" fld="5" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16 EnabledSubtotalsDefault="0" SubtotalsOnTopDefault="0"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable17.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{19D428D0-8183-46E6-BA88-0E3BE17B9AAB}" name="PivotTable4" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+  <location ref="A41:J47" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField axis="axisRow" compact="0" outline="0" showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" compact="0" outline="0" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" compact="0" outline="0" showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField compact="0" numFmtId="8" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField dataField="1" compact="0" numFmtId="8" outline="0" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="2">
+    <field x="2"/>
+    <field x="3"/>
+  </colFields>
+  <colItems count="9">
+    <i>
+      <x/>
+      <x/>
+    </i>
+    <i t="default">
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i t="default">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i t="default">
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable18.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7BBAE12B-BB3E-43CA-AA17-30B40E255BE1}" name="PivotTable3" cacheId="14" dataOnRows="1" dataPosition="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+  <location ref="A27:L37" firstHeaderRow="1" firstDataRow="3" firstDataCol="2"/>
+  <pivotFields count="7">
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField axis="axisRow" compact="0" outline="0" showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" compact="0" outline="0" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" compact="0" outline="0" showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField compact="0" numFmtId="8" outline="0" showAll="0"/>
+    <pivotField dataField="1" compact="0" outline="0" showAll="0"/>
+    <pivotField dataField="1" compact="0" numFmtId="8" outline="0" showAll="0"/>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="1"/>
+    <field x="-2"/>
+  </rowFields>
+  <rowItems count="8">
+    <i>
+      <x/>
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="1"/>
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+    <i t="grand" i="1">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="2">
+    <field x="3"/>
+    <field x="2"/>
+  </colFields>
+  <colItems count="10">
+    <i>
+      <x/>
+      <x/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i t="default">
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+      <x v="2"/>
+    </i>
+    <i t="default">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+      <x v="1"/>
+    </i>
+    <i t="default">
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+      <x v="1"/>
+    </i>
+    <i t="default">
+      <x v="3"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sum of Units Sold" fld="5" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable19.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D9A41ACB-E893-4EA3-9596-BDA8C70F2DBD}" name="PivotTable2" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+  <location ref="A16:M23" firstHeaderRow="1" firstDataRow="4" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+      </items>
+    </pivotField>
+    <pivotField compact="0" numFmtId="8" outline="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dataField="1" compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dataField="1" compact="0" numFmtId="8" outline="0" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="3">
+    <field x="2"/>
+    <field x="-2"/>
+    <field x="3"/>
+  </colFields>
+  <colItems count="12">
+    <i>
+      <x/>
+      <x/>
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+      <x/>
+      <x v="2"/>
+    </i>
+    <i r="2">
+      <x v="3"/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+      <x v="2"/>
+    </i>
+    <i r="2" i="1">
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="2"/>
+      <x/>
+      <x/>
+    </i>
+    <i r="2">
+      <x v="1"/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+      <x/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+    <i t="grand" i="1">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sum of Units Sold" fld="5" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16 EnabledSubtotalsDefault="0" SubtotalsOnTopDefault="0"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C85503F4-685C-4E34-9D3D-85E927BBC202}" name="PivotTable2" cacheId="76" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="F2:L14" firstHeaderRow="1" firstDataRow="2" firstDataCol="2"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9700D86C-9ED7-4F06-8532-1AFF8F9B1C2A}" name="PivotTable1" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A2:C13" firstHeaderRow="1" firstDataRow="1" firstDataCol="2"/>
   <pivotFields count="7">
     <pivotField showAll="0"/>
+    <pivotField axis="axisRow" outline="0" showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" outline="0" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="8" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" numFmtId="8" showAll="0"/>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="1"/>
+    <field x="2"/>
+  </rowFields>
+  <rowItems count="11">
+    <i>
+      <x/>
+      <x/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i t="default">
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i t="default">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i t="default">
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable20.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{27A0C44C-B952-4C7D-8EA3-685998630CEA}" name="PivotTable1" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+  <location ref="A1:J13" firstHeaderRow="1" firstDataRow="3" firstDataCol="2"/>
+  <pivotFields count="7">
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField axis="axisRow" compact="0" outline="0" showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" compact="0" outline="0" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" compact="0" outline="0" showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField compact="0" numFmtId="8" outline="0" showAll="0"/>
+    <pivotField dataField="1" compact="0" outline="0" showAll="0"/>
+    <pivotField dataField="1" compact="0" numFmtId="8" outline="0" showAll="0"/>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="1"/>
+    <field x="3"/>
+  </rowFields>
+  <rowItems count="10">
+    <i>
+      <x/>
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i t="default">
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+      <x/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i t="default">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+      <x/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i t="default">
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="2">
+    <field x="-2"/>
+    <field x="2"/>
+  </colFields>
+  <colItems count="8">
+    <i>
+      <x/>
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i r="1" i="1">
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+    <i t="grand" i="1">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sum of Units Sold" fld="5" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9489D35E-5C73-42E5-85C8-4C22966D7885}" name="PivotTable3" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A19:N32" firstHeaderRow="1" firstDataRow="3" firstDataCol="2"/>
+  <pivotFields count="7">
+    <pivotField axis="axisCol" showAll="0">
+      <items count="8">
+        <item x="3"/>
+        <item x="5"/>
+        <item x="4"/>
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="6"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
     <pivotField axis="axisRow" outline="0" showAll="0">
       <items count="4">
         <item x="1"/>
@@ -1748,20 +2434,46 @@
       <x/>
     </i>
   </rowItems>
-  <colFields count="1">
+  <colFields count="2">
     <field x="3"/>
+    <field x="0"/>
   </colFields>
-  <colItems count="5">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
+  <colItems count="12">
+    <i>
+      <x/>
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
+    <i t="default">
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+      <x v="4"/>
+    </i>
+    <i t="default">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+      <x v="5"/>
+    </i>
+    <i t="default">
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+      <x v="2"/>
+    </i>
+    <i t="default">
       <x v="3"/>
     </i>
     <i t="grand">
@@ -1783,12 +2495,12 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9700D86C-9ED7-4F06-8532-1AFF8F9B1C2A}" name="PivotTable1" cacheId="76" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A2:C13" firstHeaderRow="1" firstDataRow="1" firstDataCol="2"/>
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E0D468BF-C425-4EAD-A446-B2DC92F4629D}" name="PivotTable5" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A50:C68" firstHeaderRow="1" firstDataRow="1" firstDataCol="2"/>
   <pivotFields count="7">
     <pivotField showAll="0"/>
-    <pivotField axis="axisRow" outline="0" showAll="0">
+    <pivotField axis="axisRow" showAll="0">
       <items count="4">
         <item x="1"/>
         <item x="2"/>
@@ -1804,48 +2516,82 @@
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
     <pivotField numFmtId="8" showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField dataField="1" numFmtId="8" showAll="0"/>
   </pivotFields>
-  <rowFields count="2">
+  <rowFields count="3">
     <field x="1"/>
     <field x="2"/>
+    <field x="3"/>
   </rowFields>
-  <rowItems count="11">
-    <i>
-      <x/>
+  <rowItems count="18">
+    <i>
       <x/>
     </i>
     <i r="1">
-      <x v="2"/>
-    </i>
-    <i t="default">
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
+      <x/>
+      <x/>
+    </i>
+    <i t="default" r="1">
       <x/>
     </i>
     <i r="1">
+      <x v="2"/>
+      <x v="1"/>
+    </i>
+    <i t="default" r="1">
+      <x v="2"/>
+    </i>
+    <i>
       <x v="1"/>
     </i>
     <i r="1">
-      <x v="2"/>
-    </i>
-    <i t="default">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
+      <x/>
+      <x/>
+    </i>
+    <i t="default" r="1">
       <x/>
     </i>
     <i r="1">
       <x v="1"/>
-    </i>
-    <i t="default">
-      <x v="2"/>
+      <x v="3"/>
+    </i>
+    <i t="default" r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+      <x/>
+    </i>
+    <i t="default" r="1">
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x/>
+      <x/>
+    </i>
+    <i t="default" r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+      <x v="2"/>
+    </i>
+    <i t="default" r="1">
+      <x v="1"/>
     </i>
     <i t="grand">
       <x/>
@@ -1869,8 +2615,560 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{175B013F-D147-4A15-8D15-92D91BED1370}" name="PivotTable6" cacheId="76" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8E6A55A6-41F1-4A12-AA6C-1453FC01C41C}" name="PivotTable4" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="G27:P46" firstHeaderRow="1" firstDataRow="2" firstDataCol="2"/>
+  <pivotFields count="7">
+    <pivotField axis="axisCol" showAll="0">
+      <items count="8">
+        <item x="3"/>
+        <item x="5"/>
+        <item x="4"/>
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="6"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" outline="0" showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField numFmtId="8" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" numFmtId="8" showAll="0"/>
+  </pivotFields>
+  <rowFields count="3">
+    <field x="1"/>
+    <field x="2"/>
+    <field x="3"/>
+  </rowFields>
+  <rowItems count="18">
+    <i>
+      <x/>
+      <x/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="2">
+      <x v="1"/>
+    </i>
+    <i t="default">
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+      <x/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="2">
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i t="default">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+      <x/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="2">
+      <x v="2"/>
+    </i>
+    <i t="default">
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="0"/>
+  </colFields>
+  <colItems count="8">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A72C228A-931B-4AB3-96BB-CE66D2960F7F}" name="PivotTable3" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A27:C45" firstHeaderRow="1" firstDataRow="1" firstDataCol="2"/>
+  <pivotFields count="7">
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" outline="0" showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField numFmtId="8" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" numFmtId="8" showAll="0"/>
+  </pivotFields>
+  <rowFields count="3">
+    <field x="1"/>
+    <field x="2"/>
+    <field x="3"/>
+  </rowFields>
+  <rowItems count="18">
+    <i>
+      <x/>
+      <x/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="2">
+      <x v="1"/>
+    </i>
+    <i t="default">
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+      <x/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="2">
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i t="default">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+      <x/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="2">
+      <x v="2"/>
+    </i>
+    <i t="default">
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A4220495-98B6-4A94-939F-DE40F02C70FD}" name="PivotTable2" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="G2:Q21" firstHeaderRow="1" firstDataRow="2" firstDataCol="3"/>
+  <pivotFields count="7">
+    <pivotField axis="axisCol" showAll="0">
+      <items count="8">
+        <item x="3"/>
+        <item x="5"/>
+        <item x="4"/>
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="6"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" outline="0" showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" outline="0" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField numFmtId="8" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" numFmtId="8" showAll="0"/>
+  </pivotFields>
+  <rowFields count="3">
+    <field x="1"/>
+    <field x="2"/>
+    <field x="3"/>
+  </rowFields>
+  <rowItems count="18">
+    <i>
+      <x/>
+      <x/>
+      <x/>
+    </i>
+    <i t="default" r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+      <x v="1"/>
+    </i>
+    <i t="default" r="1">
+      <x v="2"/>
+    </i>
+    <i t="default">
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+      <x/>
+      <x/>
+    </i>
+    <i t="default" r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+      <x v="3"/>
+    </i>
+    <i t="default" r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+      <x/>
+    </i>
+    <i t="default" r="1">
+      <x v="2"/>
+    </i>
+    <i t="default">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+      <x/>
+      <x/>
+    </i>
+    <i t="default" r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+      <x v="2"/>
+    </i>
+    <i t="default" r="1">
+      <x v="1"/>
+    </i>
+    <i t="default">
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="0"/>
+  </colFields>
+  <colItems count="8">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable8.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A906CC5C-4FF2-45FA-A83F-8FDA62F94517}" name="PivotTable1" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A2:D20" firstHeaderRow="1" firstDataRow="1" firstDataCol="3"/>
+  <pivotFields count="7">
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" outline="0" showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" outline="0" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField numFmtId="8" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" numFmtId="8" showAll="0"/>
+  </pivotFields>
+  <rowFields count="3">
+    <field x="1"/>
+    <field x="2"/>
+    <field x="3"/>
+  </rowFields>
+  <rowItems count="18">
+    <i>
+      <x/>
+      <x/>
+      <x/>
+    </i>
+    <i t="default" r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+      <x v="1"/>
+    </i>
+    <i t="default" r="1">
+      <x v="2"/>
+    </i>
+    <i t="default">
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+      <x/>
+      <x/>
+    </i>
+    <i t="default" r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+      <x v="3"/>
+    </i>
+    <i t="default" r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+      <x/>
+    </i>
+    <i t="default" r="1">
+      <x v="2"/>
+    </i>
+    <i t="default">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+      <x/>
+      <x/>
+    </i>
+    <i t="default" r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+      <x v="2"/>
+    </i>
+    <i t="default" r="1">
+      <x v="1"/>
+    </i>
+    <i t="default">
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable9.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{175B013F-D147-4A15-8D15-92D91BED1370}" name="PivotTable6" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="G50:P69" firstHeaderRow="1" firstDataRow="2" firstDataCol="2"/>
   <pivotFields count="7">
     <pivotField axis="axisCol" showAll="0">
@@ -2010,678 +3308,6 @@
     <i t="grand">
       <x/>
     </i>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E0D468BF-C425-4EAD-A446-B2DC92F4629D}" name="PivotTable5" cacheId="76" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A50:C68" firstHeaderRow="1" firstDataRow="1" firstDataCol="2"/>
-  <pivotFields count="7">
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="4">
-        <item x="1"/>
-        <item x="2"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" outline="0" showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="5">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField numFmtId="8" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" numFmtId="8" showAll="0"/>
-  </pivotFields>
-  <rowFields count="3">
-    <field x="1"/>
-    <field x="2"/>
-    <field x="3"/>
-  </rowFields>
-  <rowItems count="18">
-    <i>
-      <x/>
-    </i>
-    <i r="1">
-      <x/>
-      <x/>
-    </i>
-    <i t="default" r="1">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="2"/>
-      <x v="1"/>
-    </i>
-    <i t="default" r="1">
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x/>
-      <x/>
-    </i>
-    <i t="default" r="1">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-      <x v="3"/>
-    </i>
-    <i t="default" r="1">
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="2"/>
-      <x/>
-    </i>
-    <i t="default" r="1">
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x/>
-      <x/>
-    </i>
-    <i t="default" r="1">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-      <x v="2"/>
-    </i>
-    <i t="default" r="1">
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8E6A55A6-41F1-4A12-AA6C-1453FC01C41C}" name="PivotTable4" cacheId="76" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="G27:P46" firstHeaderRow="1" firstDataRow="2" firstDataCol="2"/>
-  <pivotFields count="7">
-    <pivotField axis="axisCol" showAll="0">
-      <items count="8">
-        <item x="3"/>
-        <item x="5"/>
-        <item x="4"/>
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item x="6"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" outline="0" showAll="0">
-      <items count="4">
-        <item x="1"/>
-        <item x="2"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="5">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField numFmtId="8" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" numFmtId="8" showAll="0"/>
-  </pivotFields>
-  <rowFields count="3">
-    <field x="1"/>
-    <field x="2"/>
-    <field x="3"/>
-  </rowFields>
-  <rowItems count="18">
-    <i>
-      <x/>
-      <x/>
-    </i>
-    <i r="2">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="2"/>
-    </i>
-    <i r="2">
-      <x v="1"/>
-    </i>
-    <i t="default">
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-      <x/>
-    </i>
-    <i r="2">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i r="2">
-      <x v="3"/>
-    </i>
-    <i r="1">
-      <x v="2"/>
-    </i>
-    <i r="2">
-      <x/>
-    </i>
-    <i t="default">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-      <x/>
-    </i>
-    <i r="2">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i r="2">
-      <x v="2"/>
-    </i>
-    <i t="default">
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="0"/>
-  </colFields>
-  <colItems count="8">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A72C228A-931B-4AB3-96BB-CE66D2960F7F}" name="PivotTable3" cacheId="76" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A27:C45" firstHeaderRow="1" firstDataRow="1" firstDataCol="2"/>
-  <pivotFields count="7">
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" outline="0" showAll="0">
-      <items count="4">
-        <item x="1"/>
-        <item x="2"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="5">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField numFmtId="8" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" numFmtId="8" showAll="0"/>
-  </pivotFields>
-  <rowFields count="3">
-    <field x="1"/>
-    <field x="2"/>
-    <field x="3"/>
-  </rowFields>
-  <rowItems count="18">
-    <i>
-      <x/>
-      <x/>
-    </i>
-    <i r="2">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="2"/>
-    </i>
-    <i r="2">
-      <x v="1"/>
-    </i>
-    <i t="default">
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-      <x/>
-    </i>
-    <i r="2">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i r="2">
-      <x v="3"/>
-    </i>
-    <i r="1">
-      <x v="2"/>
-    </i>
-    <i r="2">
-      <x/>
-    </i>
-    <i t="default">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-      <x/>
-    </i>
-    <i r="2">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i r="2">
-      <x v="2"/>
-    </i>
-    <i t="default">
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A4220495-98B6-4A94-939F-DE40F02C70FD}" name="PivotTable2" cacheId="76" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="G2:Q21" firstHeaderRow="1" firstDataRow="2" firstDataCol="3"/>
-  <pivotFields count="7">
-    <pivotField axis="axisCol" showAll="0">
-      <items count="8">
-        <item x="3"/>
-        <item x="5"/>
-        <item x="4"/>
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item x="6"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" outline="0" showAll="0">
-      <items count="4">
-        <item x="1"/>
-        <item x="2"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" outline="0" showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="5">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField numFmtId="8" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" numFmtId="8" showAll="0"/>
-  </pivotFields>
-  <rowFields count="3">
-    <field x="1"/>
-    <field x="2"/>
-    <field x="3"/>
-  </rowFields>
-  <rowItems count="18">
-    <i>
-      <x/>
-      <x/>
-      <x/>
-    </i>
-    <i t="default" r="1">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="2"/>
-      <x v="1"/>
-    </i>
-    <i t="default" r="1">
-      <x v="2"/>
-    </i>
-    <i t="default">
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-      <x/>
-      <x/>
-    </i>
-    <i t="default" r="1">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-      <x v="3"/>
-    </i>
-    <i t="default" r="1">
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="2"/>
-      <x/>
-    </i>
-    <i t="default" r="1">
-      <x v="2"/>
-    </i>
-    <i t="default">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-      <x/>
-      <x/>
-    </i>
-    <i t="default" r="1">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-      <x v="2"/>
-    </i>
-    <i t="default" r="1">
-      <x v="1"/>
-    </i>
-    <i t="default">
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="0"/>
-  </colFields>
-  <colItems count="8">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A906CC5C-4FF2-45FA-A83F-8FDA62F94517}" name="PivotTable1" cacheId="76" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A2:D20" firstHeaderRow="1" firstDataRow="1" firstDataCol="3"/>
-  <pivotFields count="7">
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" outline="0" showAll="0">
-      <items count="4">
-        <item x="1"/>
-        <item x="2"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" outline="0" showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="5">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField numFmtId="8" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" numFmtId="8" showAll="0"/>
-  </pivotFields>
-  <rowFields count="3">
-    <field x="1"/>
-    <field x="2"/>
-    <field x="3"/>
-  </rowFields>
-  <rowItems count="18">
-    <i>
-      <x/>
-      <x/>
-      <x/>
-    </i>
-    <i t="default" r="1">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="2"/>
-      <x v="1"/>
-    </i>
-    <i t="default" r="1">
-      <x v="2"/>
-    </i>
-    <i t="default">
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-      <x/>
-      <x/>
-    </i>
-    <i t="default" r="1">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-      <x v="3"/>
-    </i>
-    <i t="default" r="1">
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="2"/>
-      <x/>
-    </i>
-    <i t="default" r="1">
-      <x v="2"/>
-    </i>
-    <i t="default">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-      <x/>
-      <x/>
-    </i>
-    <i t="default" r="1">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-      <x v="2"/>
-    </i>
-    <i t="default" r="1">
-      <x v="1"/>
-    </i>
-    <i t="default">
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
   </colItems>
   <dataFields count="1">
     <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0"/>
@@ -2998,7 +3624,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection sqref="A1:G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5513,7 +6139,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25CC9518-29E2-4301-B4B7-F8D0C84479C0}">
   <dimension ref="A1:N101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+    <sheetView topLeftCell="A67" workbookViewId="0">
       <selection activeCell="J78" sqref="J78"/>
     </sheetView>
   </sheetViews>
@@ -7636,4 +8262,1340 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3E9C459-FCCF-4AE5-9F86-7BA88974E502}">
+  <dimension ref="A1:P61"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="E61" sqref="E61"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="14" width="16" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.77734375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="20.77734375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" t="s">
+        <v>50</v>
+      </c>
+      <c r="J2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="6">
+        <v>2</v>
+      </c>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6">
+        <v>831.5</v>
+      </c>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6">
+        <v>2</v>
+      </c>
+      <c r="J4" s="6">
+        <v>831.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6">
+        <v>1</v>
+      </c>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6">
+        <v>24.99</v>
+      </c>
+      <c r="I5" s="6">
+        <v>1</v>
+      </c>
+      <c r="J5" s="6">
+        <v>24.99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="6">
+        <v>2</v>
+      </c>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6">
+        <v>1</v>
+      </c>
+      <c r="F6" s="6">
+        <v>831.5</v>
+      </c>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6">
+        <v>24.99</v>
+      </c>
+      <c r="I6" s="6">
+        <v>3</v>
+      </c>
+      <c r="J6" s="6">
+        <v>856.49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="6">
+        <v>2</v>
+      </c>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6">
+        <v>2</v>
+      </c>
+      <c r="F7" s="6">
+        <v>831.5</v>
+      </c>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6">
+        <v>831.5</v>
+      </c>
+      <c r="I7" s="6">
+        <v>4</v>
+      </c>
+      <c r="J7" s="6">
+        <v>1663</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6">
+        <v>6</v>
+      </c>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6">
+        <v>1194</v>
+      </c>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6">
+        <v>6</v>
+      </c>
+      <c r="J8" s="6">
+        <v>1194</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="6">
+        <v>2</v>
+      </c>
+      <c r="D9" s="6">
+        <v>6</v>
+      </c>
+      <c r="E9" s="6">
+        <v>2</v>
+      </c>
+      <c r="F9" s="6">
+        <v>831.5</v>
+      </c>
+      <c r="G9" s="6">
+        <v>1194</v>
+      </c>
+      <c r="H9" s="6">
+        <v>831.5</v>
+      </c>
+      <c r="I9" s="6">
+        <v>10</v>
+      </c>
+      <c r="J9" s="6">
+        <v>2857</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="6">
+        <v>1</v>
+      </c>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6">
+        <v>415.75</v>
+      </c>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6">
+        <v>1</v>
+      </c>
+      <c r="J10" s="6">
+        <v>415.75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6">
+        <v>1</v>
+      </c>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6">
+        <v>99</v>
+      </c>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6">
+        <v>1</v>
+      </c>
+      <c r="J11" s="6">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="6">
+        <v>1</v>
+      </c>
+      <c r="D12" s="6">
+        <v>1</v>
+      </c>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6">
+        <v>415.75</v>
+      </c>
+      <c r="G12" s="6">
+        <v>99</v>
+      </c>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6">
+        <v>2</v>
+      </c>
+      <c r="J12" s="6">
+        <v>514.75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="6">
+        <v>5</v>
+      </c>
+      <c r="D13" s="6">
+        <v>7</v>
+      </c>
+      <c r="E13" s="6">
+        <v>3</v>
+      </c>
+      <c r="F13" s="6">
+        <v>2078.75</v>
+      </c>
+      <c r="G13" s="6">
+        <v>1293</v>
+      </c>
+      <c r="H13" s="6">
+        <v>856.49</v>
+      </c>
+      <c r="I13" s="6">
+        <v>15</v>
+      </c>
+      <c r="J13" s="6">
+        <v>4228.24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" t="s">
+        <v>10</v>
+      </c>
+      <c r="H17" t="s">
+        <v>13</v>
+      </c>
+      <c r="L17" t="s">
+        <v>50</v>
+      </c>
+      <c r="M17" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" t="s">
+        <v>49</v>
+      </c>
+      <c r="F18" t="s">
+        <v>22</v>
+      </c>
+      <c r="H18" t="s">
+        <v>49</v>
+      </c>
+      <c r="J18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" t="s">
+        <v>16</v>
+      </c>
+      <c r="F19" t="s">
+        <v>11</v>
+      </c>
+      <c r="G19" t="s">
+        <v>16</v>
+      </c>
+      <c r="H19" t="s">
+        <v>9</v>
+      </c>
+      <c r="I19" t="s">
+        <v>14</v>
+      </c>
+      <c r="J19" t="s">
+        <v>9</v>
+      </c>
+      <c r="K19" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" s="6">
+        <v>2</v>
+      </c>
+      <c r="C20" s="6">
+        <v>831.5</v>
+      </c>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6">
+        <v>1</v>
+      </c>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6">
+        <v>24.99</v>
+      </c>
+      <c r="L20" s="6">
+        <v>3</v>
+      </c>
+      <c r="M20" s="6">
+        <v>856.49</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" s="6">
+        <v>2</v>
+      </c>
+      <c r="C21" s="6">
+        <v>831.5</v>
+      </c>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6">
+        <v>6</v>
+      </c>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6">
+        <v>1194</v>
+      </c>
+      <c r="H21" s="6">
+        <v>2</v>
+      </c>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6">
+        <v>831.5</v>
+      </c>
+      <c r="K21" s="6"/>
+      <c r="L21" s="6">
+        <v>10</v>
+      </c>
+      <c r="M21" s="6">
+        <v>2857</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" s="6">
+        <v>1</v>
+      </c>
+      <c r="C22" s="6">
+        <v>415.75</v>
+      </c>
+      <c r="D22" s="6">
+        <v>1</v>
+      </c>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6">
+        <v>99</v>
+      </c>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6"/>
+      <c r="L22" s="6">
+        <v>2</v>
+      </c>
+      <c r="M22" s="6">
+        <v>514.75</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23" s="6">
+        <v>5</v>
+      </c>
+      <c r="C23" s="6">
+        <v>2078.75</v>
+      </c>
+      <c r="D23" s="6">
+        <v>1</v>
+      </c>
+      <c r="E23" s="6">
+        <v>6</v>
+      </c>
+      <c r="F23" s="6">
+        <v>99</v>
+      </c>
+      <c r="G23" s="6">
+        <v>1194</v>
+      </c>
+      <c r="H23" s="6">
+        <v>2</v>
+      </c>
+      <c r="I23" s="6">
+        <v>1</v>
+      </c>
+      <c r="J23" s="6">
+        <v>831.5</v>
+      </c>
+      <c r="K23" s="6">
+        <v>24.99</v>
+      </c>
+      <c r="L23" s="6">
+        <v>15</v>
+      </c>
+      <c r="M23" s="6">
+        <v>4228.24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C27" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C28" t="s">
+        <v>9</v>
+      </c>
+      <c r="E28" t="s">
+        <v>29</v>
+      </c>
+      <c r="F28" t="s">
+        <v>14</v>
+      </c>
+      <c r="G28" t="s">
+        <v>30</v>
+      </c>
+      <c r="H28" t="s">
+        <v>11</v>
+      </c>
+      <c r="I28" t="s">
+        <v>31</v>
+      </c>
+      <c r="J28" t="s">
+        <v>16</v>
+      </c>
+      <c r="K28" t="s">
+        <v>32</v>
+      </c>
+      <c r="L28" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C29" t="s">
+        <v>8</v>
+      </c>
+      <c r="D29" t="s">
+        <v>13</v>
+      </c>
+      <c r="F29" t="s">
+        <v>13</v>
+      </c>
+      <c r="H29" t="s">
+        <v>10</v>
+      </c>
+      <c r="J29" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>12</v>
+      </c>
+      <c r="B30" t="s">
+        <v>49</v>
+      </c>
+      <c r="C30" s="6">
+        <v>2</v>
+      </c>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6">
+        <v>2</v>
+      </c>
+      <c r="F30" s="6">
+        <v>1</v>
+      </c>
+      <c r="G30" s="6">
+        <v>1</v>
+      </c>
+      <c r="H30" s="6"/>
+      <c r="I30" s="6"/>
+      <c r="J30" s="6"/>
+      <c r="K30" s="6"/>
+      <c r="L30" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
+        <v>22</v>
+      </c>
+      <c r="C31" s="6">
+        <v>831.5</v>
+      </c>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6">
+        <v>831.5</v>
+      </c>
+      <c r="F31" s="6">
+        <v>24.99</v>
+      </c>
+      <c r="G31" s="6">
+        <v>24.99</v>
+      </c>
+      <c r="H31" s="6"/>
+      <c r="I31" s="6"/>
+      <c r="J31" s="6"/>
+      <c r="K31" s="6"/>
+      <c r="L31" s="6">
+        <v>856.49</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>15</v>
+      </c>
+      <c r="B32" t="s">
+        <v>49</v>
+      </c>
+      <c r="C32" s="6">
+        <v>2</v>
+      </c>
+      <c r="D32" s="6">
+        <v>2</v>
+      </c>
+      <c r="E32" s="6">
+        <v>4</v>
+      </c>
+      <c r="F32" s="6"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="6"/>
+      <c r="I32" s="6"/>
+      <c r="J32" s="6">
+        <v>6</v>
+      </c>
+      <c r="K32" s="6">
+        <v>6</v>
+      </c>
+      <c r="L32" s="6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
+        <v>22</v>
+      </c>
+      <c r="C33" s="6">
+        <v>831.5</v>
+      </c>
+      <c r="D33" s="6">
+        <v>831.5</v>
+      </c>
+      <c r="E33" s="6">
+        <v>1663</v>
+      </c>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
+      <c r="I33" s="6"/>
+      <c r="J33" s="6">
+        <v>1194</v>
+      </c>
+      <c r="K33" s="6">
+        <v>1194</v>
+      </c>
+      <c r="L33" s="6">
+        <v>2857</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>7</v>
+      </c>
+      <c r="B34" t="s">
+        <v>49</v>
+      </c>
+      <c r="C34" s="6">
+        <v>1</v>
+      </c>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6">
+        <v>1</v>
+      </c>
+      <c r="F34" s="6"/>
+      <c r="G34" s="6"/>
+      <c r="H34" s="6">
+        <v>1</v>
+      </c>
+      <c r="I34" s="6">
+        <v>1</v>
+      </c>
+      <c r="J34" s="6"/>
+      <c r="K34" s="6"/>
+      <c r="L34" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B35" t="s">
+        <v>22</v>
+      </c>
+      <c r="C35" s="6">
+        <v>415.75</v>
+      </c>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6">
+        <v>415.75</v>
+      </c>
+      <c r="F35" s="6"/>
+      <c r="G35" s="6"/>
+      <c r="H35" s="6">
+        <v>99</v>
+      </c>
+      <c r="I35" s="6">
+        <v>99</v>
+      </c>
+      <c r="J35" s="6"/>
+      <c r="K35" s="6"/>
+      <c r="L35" s="6">
+        <v>514.75</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>50</v>
+      </c>
+      <c r="C36" s="6">
+        <v>5</v>
+      </c>
+      <c r="D36" s="6">
+        <v>2</v>
+      </c>
+      <c r="E36" s="6">
+        <v>7</v>
+      </c>
+      <c r="F36" s="6">
+        <v>1</v>
+      </c>
+      <c r="G36" s="6">
+        <v>1</v>
+      </c>
+      <c r="H36" s="6">
+        <v>1</v>
+      </c>
+      <c r="I36" s="6">
+        <v>1</v>
+      </c>
+      <c r="J36" s="6">
+        <v>6</v>
+      </c>
+      <c r="K36" s="6">
+        <v>6</v>
+      </c>
+      <c r="L36" s="6">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>51</v>
+      </c>
+      <c r="C37" s="6">
+        <v>2078.75</v>
+      </c>
+      <c r="D37" s="6">
+        <v>831.5</v>
+      </c>
+      <c r="E37" s="6">
+        <v>2910.25</v>
+      </c>
+      <c r="F37" s="6">
+        <v>24.99</v>
+      </c>
+      <c r="G37" s="6">
+        <v>24.99</v>
+      </c>
+      <c r="H37" s="6">
+        <v>99</v>
+      </c>
+      <c r="I37" s="6">
+        <v>99</v>
+      </c>
+      <c r="J37" s="6">
+        <v>1194</v>
+      </c>
+      <c r="K37" s="6">
+        <v>1194</v>
+      </c>
+      <c r="L37" s="6">
+        <v>4228.24</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A41" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B42" t="s">
+        <v>8</v>
+      </c>
+      <c r="C42" t="s">
+        <v>24</v>
+      </c>
+      <c r="D42" t="s">
+        <v>10</v>
+      </c>
+      <c r="F42" t="s">
+        <v>26</v>
+      </c>
+      <c r="G42" t="s">
+        <v>13</v>
+      </c>
+      <c r="I42" t="s">
+        <v>25</v>
+      </c>
+      <c r="J42" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A43" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B43" t="s">
+        <v>9</v>
+      </c>
+      <c r="D43" t="s">
+        <v>11</v>
+      </c>
+      <c r="E43" t="s">
+        <v>16</v>
+      </c>
+      <c r="G43" t="s">
+        <v>9</v>
+      </c>
+      <c r="H43" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>12</v>
+      </c>
+      <c r="B44" s="6">
+        <v>831.5</v>
+      </c>
+      <c r="C44" s="6">
+        <v>831.5</v>
+      </c>
+      <c r="D44" s="6"/>
+      <c r="E44" s="6"/>
+      <c r="F44" s="6"/>
+      <c r="G44" s="6"/>
+      <c r="H44" s="6">
+        <v>24.99</v>
+      </c>
+      <c r="I44" s="6">
+        <v>24.99</v>
+      </c>
+      <c r="J44" s="6">
+        <v>856.49</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>15</v>
+      </c>
+      <c r="B45" s="6">
+        <v>831.5</v>
+      </c>
+      <c r="C45" s="6">
+        <v>831.5</v>
+      </c>
+      <c r="D45" s="6"/>
+      <c r="E45" s="6">
+        <v>1194</v>
+      </c>
+      <c r="F45" s="6">
+        <v>1194</v>
+      </c>
+      <c r="G45" s="6">
+        <v>831.5</v>
+      </c>
+      <c r="H45" s="6"/>
+      <c r="I45" s="6">
+        <v>831.5</v>
+      </c>
+      <c r="J45" s="6">
+        <v>2857</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>7</v>
+      </c>
+      <c r="B46" s="6">
+        <v>415.75</v>
+      </c>
+      <c r="C46" s="6">
+        <v>415.75</v>
+      </c>
+      <c r="D46" s="6">
+        <v>99</v>
+      </c>
+      <c r="E46" s="6"/>
+      <c r="F46" s="6">
+        <v>99</v>
+      </c>
+      <c r="G46" s="6"/>
+      <c r="H46" s="6"/>
+      <c r="I46" s="6"/>
+      <c r="J46" s="6">
+        <v>514.75</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>18</v>
+      </c>
+      <c r="B47" s="6">
+        <v>2078.75</v>
+      </c>
+      <c r="C47" s="6">
+        <v>2078.75</v>
+      </c>
+      <c r="D47" s="6">
+        <v>99</v>
+      </c>
+      <c r="E47" s="6">
+        <v>1194</v>
+      </c>
+      <c r="F47" s="6">
+        <v>1293</v>
+      </c>
+      <c r="G47" s="6">
+        <v>831.5</v>
+      </c>
+      <c r="H47" s="6">
+        <v>24.99</v>
+      </c>
+      <c r="I47" s="6">
+        <v>856.49</v>
+      </c>
+      <c r="J47" s="6">
+        <v>4228.24</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="C50" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="C51" t="s">
+        <v>22</v>
+      </c>
+      <c r="I51" t="s">
+        <v>49</v>
+      </c>
+      <c r="O51" t="s">
+        <v>51</v>
+      </c>
+      <c r="P51" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="C52" t="s">
+        <v>12</v>
+      </c>
+      <c r="E52" t="s">
+        <v>15</v>
+      </c>
+      <c r="G52" t="s">
+        <v>7</v>
+      </c>
+      <c r="I52" t="s">
+        <v>12</v>
+      </c>
+      <c r="K52" t="s">
+        <v>15</v>
+      </c>
+      <c r="M52" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A53" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C53" t="s">
+        <v>9</v>
+      </c>
+      <c r="D53" t="s">
+        <v>14</v>
+      </c>
+      <c r="E53" t="s">
+        <v>9</v>
+      </c>
+      <c r="F53" t="s">
+        <v>16</v>
+      </c>
+      <c r="G53" t="s">
+        <v>9</v>
+      </c>
+      <c r="H53" t="s">
+        <v>11</v>
+      </c>
+      <c r="I53" t="s">
+        <v>9</v>
+      </c>
+      <c r="J53" t="s">
+        <v>14</v>
+      </c>
+      <c r="K53" t="s">
+        <v>9</v>
+      </c>
+      <c r="L53" t="s">
+        <v>16</v>
+      </c>
+      <c r="M53" t="s">
+        <v>9</v>
+      </c>
+      <c r="N53" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>20100007</v>
+      </c>
+      <c r="B54" t="s">
+        <v>8</v>
+      </c>
+      <c r="C54" s="6">
+        <v>831.5</v>
+      </c>
+      <c r="D54" s="6"/>
+      <c r="E54" s="6"/>
+      <c r="F54" s="6"/>
+      <c r="G54" s="6"/>
+      <c r="H54" s="6"/>
+      <c r="I54" s="6">
+        <v>2</v>
+      </c>
+      <c r="J54" s="6"/>
+      <c r="K54" s="6"/>
+      <c r="L54" s="6"/>
+      <c r="M54" s="6"/>
+      <c r="N54" s="6"/>
+      <c r="O54" s="6">
+        <v>831.5</v>
+      </c>
+      <c r="P54" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>20100017</v>
+      </c>
+      <c r="B55" t="s">
+        <v>13</v>
+      </c>
+      <c r="C55" s="6"/>
+      <c r="D55" s="6"/>
+      <c r="E55" s="6">
+        <v>831.5</v>
+      </c>
+      <c r="F55" s="6"/>
+      <c r="G55" s="6"/>
+      <c r="H55" s="6"/>
+      <c r="I55" s="6"/>
+      <c r="J55" s="6"/>
+      <c r="K55" s="6">
+        <v>2</v>
+      </c>
+      <c r="L55" s="6"/>
+      <c r="M55" s="6"/>
+      <c r="N55" s="6"/>
+      <c r="O55" s="6">
+        <v>831.5</v>
+      </c>
+      <c r="P55" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>20100070</v>
+      </c>
+      <c r="B56" t="s">
+        <v>10</v>
+      </c>
+      <c r="C56" s="6"/>
+      <c r="D56" s="6"/>
+      <c r="E56" s="6"/>
+      <c r="F56" s="6">
+        <v>1194</v>
+      </c>
+      <c r="G56" s="6"/>
+      <c r="H56" s="6"/>
+      <c r="I56" s="6"/>
+      <c r="J56" s="6"/>
+      <c r="K56" s="6"/>
+      <c r="L56" s="6">
+        <v>6</v>
+      </c>
+      <c r="M56" s="6"/>
+      <c r="N56" s="6"/>
+      <c r="O56" s="6">
+        <v>1194</v>
+      </c>
+      <c r="P56" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>20100076</v>
+      </c>
+      <c r="B57" t="s">
+        <v>8</v>
+      </c>
+      <c r="C57" s="6"/>
+      <c r="D57" s="6"/>
+      <c r="E57" s="6"/>
+      <c r="F57" s="6"/>
+      <c r="G57" s="6">
+        <v>415.75</v>
+      </c>
+      <c r="H57" s="6"/>
+      <c r="I57" s="6"/>
+      <c r="J57" s="6"/>
+      <c r="K57" s="6"/>
+      <c r="L57" s="6"/>
+      <c r="M57" s="6">
+        <v>1</v>
+      </c>
+      <c r="N57" s="6"/>
+      <c r="O57" s="6">
+        <v>415.75</v>
+      </c>
+      <c r="P57" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>20100083</v>
+      </c>
+      <c r="B58" t="s">
+        <v>13</v>
+      </c>
+      <c r="C58" s="6"/>
+      <c r="D58" s="6">
+        <v>24.99</v>
+      </c>
+      <c r="E58" s="6"/>
+      <c r="F58" s="6"/>
+      <c r="G58" s="6"/>
+      <c r="H58" s="6"/>
+      <c r="I58" s="6"/>
+      <c r="J58" s="6">
+        <v>1</v>
+      </c>
+      <c r="K58" s="6"/>
+      <c r="L58" s="6"/>
+      <c r="M58" s="6"/>
+      <c r="N58" s="6"/>
+      <c r="O58" s="6">
+        <v>24.99</v>
+      </c>
+      <c r="P58" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>20100085</v>
+      </c>
+      <c r="B59" t="s">
+        <v>10</v>
+      </c>
+      <c r="C59" s="6"/>
+      <c r="D59" s="6"/>
+      <c r="E59" s="6"/>
+      <c r="F59" s="6"/>
+      <c r="G59" s="6"/>
+      <c r="H59" s="6">
+        <v>99</v>
+      </c>
+      <c r="I59" s="6"/>
+      <c r="J59" s="6"/>
+      <c r="K59" s="6"/>
+      <c r="L59" s="6"/>
+      <c r="M59" s="6"/>
+      <c r="N59" s="6">
+        <v>1</v>
+      </c>
+      <c r="O59" s="6">
+        <v>99</v>
+      </c>
+      <c r="P59" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>20100090</v>
+      </c>
+      <c r="B60" t="s">
+        <v>8</v>
+      </c>
+      <c r="C60" s="6"/>
+      <c r="D60" s="6"/>
+      <c r="E60" s="6">
+        <v>831.5</v>
+      </c>
+      <c r="F60" s="6"/>
+      <c r="G60" s="6"/>
+      <c r="H60" s="6"/>
+      <c r="I60" s="6"/>
+      <c r="J60" s="6"/>
+      <c r="K60" s="6">
+        <v>2</v>
+      </c>
+      <c r="L60" s="6"/>
+      <c r="M60" s="6"/>
+      <c r="N60" s="6"/>
+      <c r="O60" s="6">
+        <v>831.5</v>
+      </c>
+      <c r="P60" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>18</v>
+      </c>
+      <c r="C61" s="6">
+        <v>831.5</v>
+      </c>
+      <c r="D61" s="6">
+        <v>24.99</v>
+      </c>
+      <c r="E61" s="6">
+        <v>1663</v>
+      </c>
+      <c r="F61" s="6">
+        <v>1194</v>
+      </c>
+      <c r="G61" s="6">
+        <v>415.75</v>
+      </c>
+      <c r="H61" s="6">
+        <v>99</v>
+      </c>
+      <c r="I61" s="6">
+        <v>2</v>
+      </c>
+      <c r="J61" s="6">
+        <v>1</v>
+      </c>
+      <c r="K61" s="6">
+        <v>4</v>
+      </c>
+      <c r="L61" s="6">
+        <v>6</v>
+      </c>
+      <c r="M61" s="6">
+        <v>1</v>
+      </c>
+      <c r="N61" s="6">
+        <v>1</v>
+      </c>
+      <c r="O61" s="6">
+        <v>4228.24</v>
+      </c>
+      <c r="P61" s="6">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>